<commit_message>
excel sheets added data validation and sumifs
</commit_message>
<xml_diff>
--- a/All Practice Files.xlsx
+++ b/All Practice Files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cadd Mentor\Student_Class_Code\Jazaul_Hasan_Data_Anylytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978A445E-D8AC-4AC3-9FB1-8AAAC9C39FCA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02BA023-3DB7-4B50-B3A1-1C6D77A30345}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="797" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="797" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 1 Practice" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="319">
   <si>
     <t>Sr No.</t>
   </si>
@@ -946,6 +946,48 @@
   </si>
   <si>
     <t>fchvjj</t>
+  </si>
+  <si>
+    <t>Bhuwan Total</t>
+  </si>
+  <si>
+    <t>Harsh Total</t>
+  </si>
+  <si>
+    <t>Jayprakash Total</t>
+  </si>
+  <si>
+    <t>Kabir Total</t>
+  </si>
+  <si>
+    <t>Mahesh Total</t>
+  </si>
+  <si>
+    <t>Monu Total</t>
+  </si>
+  <si>
+    <t>Suresh Total</t>
+  </si>
+  <si>
+    <t>Dharmesh Total</t>
+  </si>
+  <si>
+    <t>Nikumbh Total</t>
+  </si>
+  <si>
+    <t>Nitin Total</t>
+  </si>
+  <si>
+    <t>Rajesh Total</t>
+  </si>
+  <si>
+    <t>Shivam Total</t>
+  </si>
+  <si>
+    <t>Sonu Total</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
   </si>
 </sst>
 </file>
@@ -956,7 +998,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1023,8 +1065,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1072,8 +1122,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1177,19 +1233,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1200,52 +1243,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1280,16 +1277,13 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1312,33 +1306,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="4" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1346,6 +1313,57 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="60% - Accent4" xfId="3" builtinId="44"/>
@@ -1354,7 +1372,7 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1373,144 +1391,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1525,23 +1405,6 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DFE54489-F036-4BF7-B080-8BEB07E11573}" name="Table1" displayName="Table1" ref="A13:C73" totalsRowShown="0" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
-  <autoFilter ref="A13:C73" xr:uid="{EEFE66AA-9069-45D9-BBFA-7CA8E4F38D32}"/>
-  <sortState ref="A14:C73">
-    <sortCondition ref="A14:A73"/>
-    <sortCondition ref="B14:B73"/>
-    <sortCondition ref="C14:C73"/>
-  </sortState>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D62B31A7-9F57-48FB-AC8E-B453891496D6}" name="Staff" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{87D3CBF4-0A52-4E35-BA5D-608E074D31C9}" name="Department" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{A009BD6B-B3C7-4F53-A1B5-4FF72803419A}" name="Sales" dataDxfId="2" dataCellStyle="Comma"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DCC9872C-5CD0-4AB7-AFA1-DEEE88E23C5D}" name="Table2" displayName="Table2" ref="A1:I44" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:I44" xr:uid="{93E7FF62-FF60-470D-9103-595FBBCCD11C}"/>
   <tableColumns count="9">
@@ -1824,7 +1687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection sqref="A1:G36"/>
     </sheetView>
   </sheetViews>
@@ -1840,19 +1703,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2856,585 +2719,585 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
+      <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13">
+      <c r="A3" s="12">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
+      <c r="A4" s="12">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
+      <c r="A5" s="12">
         <v>4</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15" t="s">
+      <c r="D5" s="13"/>
+      <c r="E5" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13">
+      <c r="A6" s="12">
         <v>5</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15" t="s">
+      <c r="D6" s="13"/>
+      <c r="E6" s="14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13">
+      <c r="A7" s="12">
         <v>6</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15" t="s">
+      <c r="D7" s="13"/>
+      <c r="E7" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13">
+      <c r="A8" s="12">
         <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
+      <c r="A9" s="12">
         <v>8</v>
       </c>
       <c r="C9" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="14" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13">
+      <c r="A10" s="12">
         <v>9</v>
       </c>
       <c r="C10" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13">
+      <c r="A11" s="12">
         <v>10</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="14" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13">
+      <c r="A12" s="12">
         <v>11</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13">
+      <c r="A13" s="12">
         <v>12</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="14" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13">
+      <c r="A14" s="12">
         <v>13</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="14" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13">
+      <c r="A15" s="12">
         <v>14</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="14" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13">
+      <c r="A16" s="12">
         <v>15</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="14" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13">
+      <c r="A17" s="12">
         <v>16</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="14" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13">
+      <c r="A18" s="12">
         <v>17</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="14" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="13">
+      <c r="A19" s="12">
         <v>18</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="14" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="13">
+      <c r="A20" s="12">
         <v>19</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="14" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="13">
+      <c r="A21" s="12">
         <v>20</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="14" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="13">
+      <c r="A22" s="12">
         <v>21</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="E22" s="21" t="s">
+      <c r="E22" s="20" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="13">
+      <c r="A23" s="12">
         <v>22</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="21" t="s">
+      <c r="E23" s="20" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="13">
+      <c r="A24" s="12">
         <v>23</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D24" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="E24" s="21" t="s">
+      <c r="E24" s="20" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="13">
+      <c r="A25" s="12">
         <v>24</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="E25" s="20" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="13">
+      <c r="A26" s="12">
         <v>25</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D26" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="E26" s="20" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="13">
+      <c r="A27" s="12">
         <v>26</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="E27" s="20" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="13">
+      <c r="A28" s="12">
         <v>27</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="14" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="13">
+      <c r="A29" s="12">
         <v>28</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="14" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="13">
+      <c r="A30" s="12">
         <v>29</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="14" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="13">
+      <c r="A31" s="12">
         <v>30</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="E31" s="15" t="s">
+      <c r="E31" s="14" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="13">
+      <c r="A32" s="12">
         <v>31</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="C32" s="22" t="s">
+      <c r="C32" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="E32" s="14" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="13">
+      <c r="A33" s="12">
         <v>32</v>
       </c>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="14" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="13">
+      <c r="A34" s="12">
         <v>33</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="14" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="13">
+      <c r="A35" s="12">
         <v>34</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="E35" s="14" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="16">
+      <c r="A36" s="15">
         <v>35</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="C36" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="D36" s="17" t="s">
+      <c r="D36" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="E36" s="18" t="s">
+      <c r="E36" s="17" t="s">
         <v>142</v>
       </c>
     </row>
@@ -3446,17 +3309,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86653973-EB28-47CE-9245-ABB5D98B25FC}">
-  <dimension ref="A1:H73"/>
+  <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.77734375" bestFit="1" customWidth="1"/>
@@ -3654,706 +3517,863 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="24"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="29" t="s">
         <v>191</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="30" t="s">
         <v>192</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="31" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="32" t="s">
         <v>200</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="34">
         <v>3430</v>
       </c>
-      <c r="H14" s="23"/>
+      <c r="H14" s="22"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="35" t="s">
         <v>200</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="37">
         <v>5123</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="32" t="s">
         <v>200</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="34">
         <v>8834</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="41" t="s">
+        <v>305</v>
+      </c>
+      <c r="B17" s="33"/>
+      <c r="C17" s="34">
+        <f>SUBTOTAL(9,C14:C16)</f>
+        <v>17387</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="B18" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C18" s="37">
+        <v>5434</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="C19" s="34">
+        <v>6072</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="B20" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C20" s="37">
+        <v>6663</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="C21" s="34">
+        <v>8277</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="41" t="s">
+        <v>306</v>
+      </c>
+      <c r="B22" s="33"/>
+      <c r="C22" s="34">
+        <f>SUBTOTAL(9,C18:C21)</f>
+        <v>26446</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="35" t="s">
+        <v>203</v>
+      </c>
+      <c r="B23" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C23" s="37">
+        <v>4578</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="C24" s="34">
+        <v>6140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="35" t="s">
+        <v>203</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C25" s="37">
+        <v>6182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="B26" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="C26" s="34">
+        <v>8280</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="41" t="s">
+        <v>307</v>
+      </c>
+      <c r="B27" s="33"/>
+      <c r="C27" s="34">
+        <f>SUBTOTAL(9,C23:C26)</f>
+        <v>25180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="35" t="s">
+        <v>201</v>
+      </c>
+      <c r="B28" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C28" s="37">
+        <v>5123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="C29" s="34">
+        <v>5177</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="35" t="s">
+        <v>201</v>
+      </c>
+      <c r="B30" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C30" s="37">
+        <v>6840</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="B31" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="C31" s="34">
+        <v>9182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="41" t="s">
+        <v>308</v>
+      </c>
+      <c r="B32" s="33"/>
+      <c r="C32" s="34">
+        <f>SUBTOTAL(9,C28:C31)</f>
+        <v>26322</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="B33" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C33" s="37">
+        <v>2707</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="B34" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="C34" s="34">
+        <v>4431</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="B35" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C35" s="37">
+        <v>5634</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="B36" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="C36" s="34">
+        <v>8291</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="41" t="s">
+        <v>309</v>
+      </c>
+      <c r="B37" s="33"/>
+      <c r="C37" s="34">
+        <f>SUBTOTAL(9,C33:C36)</f>
+        <v>21063</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="B38" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C38" s="37">
+        <v>4130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="B39" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="C39" s="34">
+        <v>5183</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="B40" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C40" s="37">
+        <v>5708</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="B41" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="C41" s="34">
+        <v>6198</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="41" t="s">
+        <v>310</v>
+      </c>
+      <c r="B42" s="33"/>
+      <c r="C42" s="34">
+        <f>SUBTOTAL(9,C38:C41)</f>
+        <v>21219</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="B43" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C43" s="37">
+        <v>2994</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="B44" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="C44" s="34">
+        <v>5111</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="B45" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C45" s="37">
+        <v>7698</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="B46" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="C46" s="34">
+        <v>8945</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="41" t="s">
+        <v>311</v>
+      </c>
+      <c r="B47" s="33"/>
+      <c r="C47" s="34">
+        <f>SUBTOTAL(9,C43:C46)</f>
+        <v>24748</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="35" t="s">
         <v>200</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B48" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="C17" s="27">
+      <c r="C48" s="37">
         <v>5925</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="26" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="42" t="s">
+        <v>305</v>
+      </c>
+      <c r="B49" s="36"/>
+      <c r="C49" s="37">
+        <f>SUBTOTAL(9,C48:C48)</f>
+        <v>5925</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B50" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="C18" s="27">
+      <c r="C50" s="34">
         <v>3295</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="26" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B51" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="C19" s="27">
+      <c r="C51" s="37">
         <v>7380</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="26" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B52" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="C20" s="27">
+      <c r="C52" s="34">
         <v>8338</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="26" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B53" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="C21" s="27">
+      <c r="C53" s="37">
         <v>9036</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C22" s="27">
-        <v>5434</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C23" s="27">
-        <v>6072</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C24" s="27">
-        <v>6663</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C25" s="27">
-        <v>8277</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="26" t="s">
-        <v>203</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C26" s="27">
-        <v>4578</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="26" t="s">
-        <v>203</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C27" s="27">
-        <v>6140</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="26" t="s">
-        <v>203</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C28" s="27">
-        <v>6182</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="26" t="s">
-        <v>203</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C29" s="27">
-        <v>8280</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="26" t="s">
-        <v>201</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C30" s="27">
-        <v>5123</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="26" t="s">
-        <v>201</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C31" s="27">
-        <v>5177</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="26" t="s">
-        <v>201</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C32" s="27">
-        <v>6840</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="26" t="s">
-        <v>201</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C33" s="27">
-        <v>9182</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="25" t="s">
-        <v>186</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C34" s="27">
-        <v>2707</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="25" t="s">
-        <v>186</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C35" s="27">
-        <v>4431</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="25" t="s">
-        <v>186</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C36" s="27">
-        <v>5634</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="25" t="s">
-        <v>186</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C37" s="27">
-        <v>8291</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C38" s="27">
-        <v>4130</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C39" s="27">
-        <v>5183</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C40" s="27">
-        <v>5708</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C41" s="27">
-        <v>6198</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="26" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="42" t="s">
+        <v>312</v>
+      </c>
+      <c r="B54" s="36"/>
+      <c r="C54" s="37">
+        <f>SUBTOTAL(9,C50:C53)</f>
+        <v>28049</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B55" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="C42" s="27">
+      <c r="C55" s="34">
         <v>3812</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="26" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="35" t="s">
         <v>202</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B56" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="C43" s="27">
+      <c r="C56" s="37">
         <v>6393</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="26" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B57" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="C44" s="27">
+      <c r="C57" s="34">
         <v>9100</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="26" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="35" t="s">
         <v>202</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B58" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="C45" s="27">
+      <c r="C58" s="37">
         <v>9262</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="26" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="42" t="s">
+        <v>313</v>
+      </c>
+      <c r="B59" s="36"/>
+      <c r="C59" s="37">
+        <f>SUBTOTAL(9,C55:C58)</f>
+        <v>28567</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="32" t="s">
         <v>196</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B60" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="C46" s="27">
+      <c r="C60" s="34">
         <v>6009</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="26" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="35" t="s">
         <v>196</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B61" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="C47" s="27">
+      <c r="C61" s="37">
         <v>6169</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="26" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="32" t="s">
         <v>196</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B62" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="C48" s="27">
+      <c r="C62" s="34">
         <v>6356</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="26" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="35" t="s">
         <v>196</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B63" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="C49" s="27">
+      <c r="C63" s="37">
         <v>6522</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="25" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="42" t="s">
+        <v>314</v>
+      </c>
+      <c r="B64" s="36"/>
+      <c r="C64" s="37">
+        <f>SUBTOTAL(9,C60:C63)</f>
+        <v>25056</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="32" t="s">
         <v>185</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B65" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="C50" s="27">
+      <c r="C65" s="34">
         <v>5178</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="25" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="35" t="s">
         <v>185</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B66" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="C51" s="27">
+      <c r="C66" s="37">
         <v>6796</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="25" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="32" t="s">
         <v>185</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B67" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="C52" s="27">
+      <c r="C67" s="34">
         <v>7961</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="25" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="35" t="s">
         <v>185</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B68" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="C53" s="27">
+      <c r="C68" s="37">
         <v>8464</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="26" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="42" t="s">
+        <v>315</v>
+      </c>
+      <c r="B69" s="36"/>
+      <c r="C69" s="37">
+        <f>SUBTOTAL(9,C65:C68)</f>
+        <v>28399</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B70" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="C54" s="27">
+      <c r="C70" s="34">
         <v>3868</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="26" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B71" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="C55" s="27">
+      <c r="C71" s="37">
         <v>4058</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="26" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B72" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="C56" s="27">
+      <c r="C72" s="34">
         <v>6651</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="26" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B73" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="C57" s="27">
+      <c r="C73" s="37">
         <v>7431</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="26" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="42" t="s">
+        <v>316</v>
+      </c>
+      <c r="B74" s="36"/>
+      <c r="C74" s="37">
+        <f>SUBTOTAL(9,C70:C73)</f>
+        <v>22008</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="32" t="s">
         <v>197</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B75" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="C58" s="27">
+      <c r="C75" s="34">
         <v>2810</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="26" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="35" t="s">
         <v>197</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B76" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="C59" s="27">
+      <c r="C76" s="37">
         <v>3114</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="26" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="32" t="s">
         <v>197</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B77" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="C60" s="27">
+      <c r="C77" s="34">
         <v>6005</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="26" t="s">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="35" t="s">
         <v>197</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B78" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="C61" s="27">
+      <c r="C78" s="37">
         <v>6565</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="25" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="42" t="s">
+        <v>317</v>
+      </c>
+      <c r="B79" s="36"/>
+      <c r="C79" s="37">
+        <f>SUBTOTAL(9,C75:C78)</f>
+        <v>18494</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="32" t="s">
         <v>187</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C62" s="27">
-        <v>2994</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="25" t="s">
+      <c r="B80" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="C80" s="34">
+        <v>3766</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="35" t="s">
         <v>187</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C63" s="27">
-        <v>5111</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="25" t="s">
+      <c r="B81" s="36" t="s">
+        <v>194</v>
+      </c>
+      <c r="C81" s="37">
+        <v>5021</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="32" t="s">
         <v>187</v>
       </c>
-      <c r="B64" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C64" s="27">
-        <v>7698</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="25" t="s">
+      <c r="B82" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="C82" s="34">
+        <v>6089</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="35" t="s">
         <v>187</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C65" s="27">
-        <v>8945</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="25" t="s">
+      <c r="B83" s="36" t="s">
+        <v>194</v>
+      </c>
+      <c r="C83" s="37">
+        <v>6368</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="32" t="s">
         <v>187</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B84" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="C66" s="27">
-        <v>3766</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="25" t="s">
+      <c r="C84" s="34">
+        <v>6968</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="35" t="s">
         <v>187</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B85" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="C67" s="27">
-        <v>5021</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="25" t="s">
+      <c r="C85" s="37">
+        <v>7317</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="32" t="s">
         <v>187</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B86" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="C68" s="27">
-        <v>6089</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="25" t="s">
+      <c r="C86" s="34">
+        <v>8429</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="38" t="s">
         <v>187</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B87" s="39" t="s">
         <v>194</v>
       </c>
-      <c r="C69" s="27">
-        <v>6368</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C70" s="27">
-        <v>6968</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C71" s="27">
-        <v>7317</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C72" s="27">
-        <v>8429</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="33" t="s">
-        <v>187</v>
-      </c>
-      <c r="B73" s="31" t="s">
-        <v>194</v>
-      </c>
-      <c r="C73" s="32">
+      <c r="C87" s="40">
         <v>8575</v>
       </c>
     </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="45" t="s">
+        <v>311</v>
+      </c>
+      <c r="B88" s="43"/>
+      <c r="C88" s="44">
+        <f>SUBTOTAL(9,C80:C87)</f>
+        <v>52533</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="45" t="s">
+        <v>318</v>
+      </c>
+      <c r="B89" s="43"/>
+      <c r="C89" s="44">
+        <f>SUBTOTAL(9,C14:C87)</f>
+        <v>371396</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A14:C73">
+  <sortState ref="A14:C87">
     <sortCondition ref="B14"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -4379,34 +4399,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="J1" s="6"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
@@ -4462,7 +4482,7 @@
       <c r="H3">
         <v>375</v>
       </c>
-      <c r="I3" s="34" t="s">
+      <c r="I3" s="24" t="s">
         <v>156</v>
       </c>
     </row>
@@ -4549,7 +4569,7 @@
       <c r="H6">
         <v>2000</v>
       </c>
-      <c r="I6" s="34" t="s">
+      <c r="I6" s="24" t="s">
         <v>156</v>
       </c>
     </row>
@@ -4723,7 +4743,7 @@
       <c r="H12">
         <v>3627</v>
       </c>
-      <c r="I12" s="34" t="s">
+      <c r="I12" s="24" t="s">
         <v>156</v>
       </c>
     </row>
@@ -4897,7 +4917,7 @@
       <c r="H18">
         <v>14000</v>
       </c>
-      <c r="I18" s="34" t="s">
+      <c r="I18" s="24" t="s">
         <v>156</v>
       </c>
     </row>
@@ -5071,7 +5091,7 @@
       <c r="H24">
         <v>21600</v>
       </c>
-      <c r="I24" s="34" t="s">
+      <c r="I24" s="24" t="s">
         <v>156</v>
       </c>
     </row>
@@ -5129,7 +5149,7 @@
       <c r="H26">
         <v>25000</v>
       </c>
-      <c r="I26" s="34" t="s">
+      <c r="I26" s="24" t="s">
         <v>156</v>
       </c>
     </row>
@@ -5158,7 +5178,7 @@
       <c r="H27">
         <v>28500</v>
       </c>
-      <c r="I27" s="34" t="s">
+      <c r="I27" s="24" t="s">
         <v>156</v>
       </c>
     </row>
@@ -5187,7 +5207,7 @@
       <c r="H28">
         <v>30000</v>
       </c>
-      <c r="I28" s="34" t="s">
+      <c r="I28" s="24" t="s">
         <v>156</v>
       </c>
     </row>
@@ -5245,7 +5265,7 @@
       <c r="H30">
         <v>38336</v>
       </c>
-      <c r="I30" s="34" t="s">
+      <c r="I30" s="24" t="s">
         <v>156</v>
       </c>
     </row>
@@ -5274,7 +5294,7 @@
       <c r="H31">
         <v>40000</v>
       </c>
-      <c r="I31" s="34" t="s">
+      <c r="I31" s="24" t="s">
         <v>156</v>
       </c>
     </row>
@@ -5419,7 +5439,7 @@
       <c r="H36">
         <v>47000</v>
       </c>
-      <c r="I36" s="34" t="s">
+      <c r="I36" s="24" t="s">
         <v>156</v>
       </c>
     </row>
@@ -5593,7 +5613,7 @@
       <c r="H42">
         <v>107820</v>
       </c>
-      <c r="I42" s="34" t="s">
+      <c r="I42" s="24" t="s">
         <v>156</v>
       </c>
     </row>
@@ -5674,7 +5694,7 @@
   <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5693,37 +5713,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>215</v>
       </c>
     </row>
@@ -5742,7 +5762,7 @@
         <f>PRODUCT(A2:B2)</f>
         <v>144</v>
       </c>
-      <c r="E2" s="35">
+      <c r="E2" s="25">
         <f>A2/B2</f>
         <v>0.5625</v>
       </c>
@@ -5758,10 +5778,10 @@
         <f>POWER(A2,3)</f>
         <v>729</v>
       </c>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="36"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -5778,7 +5798,7 @@
         <f t="shared" ref="D3:D23" si="0">PRODUCT(A3:B3)</f>
         <v>70</v>
       </c>
-      <c r="E3" s="35">
+      <c r="E3" s="25">
         <f t="shared" ref="E3:E23" si="1">A3/B3</f>
         <v>0.7</v>
       </c>
@@ -5794,10 +5814,10 @@
         <f t="shared" ref="H3:H23" si="4">POWER(A3,3)</f>
         <v>343</v>
       </c>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="36"/>
-      <c r="S3" s="36"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="26"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -5814,7 +5834,7 @@
         <f t="shared" si="0"/>
         <v>154</v>
       </c>
-      <c r="E4" s="35">
+      <c r="E4" s="25">
         <f t="shared" si="1"/>
         <v>0.7857142857142857</v>
       </c>
@@ -5834,10 +5854,10 @@
         <f>AVERAGE(A2:A6)</f>
         <v>10.6</v>
       </c>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="36"/>
-      <c r="S4" s="36"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -5854,7 +5874,7 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="E5" s="35">
+      <c r="E5" s="25">
         <f t="shared" si="1"/>
         <v>2.4</v>
       </c>
@@ -5874,10 +5894,10 @@
         <f>MIN(B4:B12)</f>
         <v>5</v>
       </c>
-      <c r="P5" s="36"/>
-      <c r="Q5" s="36"/>
-      <c r="R5" s="36"/>
-      <c r="S5" s="36"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -5894,7 +5914,7 @@
         <f t="shared" si="0"/>
         <v>224</v>
       </c>
-      <c r="E6" s="35">
+      <c r="E6" s="25">
         <f t="shared" si="1"/>
         <v>0.875</v>
       </c>
@@ -5926,7 +5946,7 @@
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="25">
         <f t="shared" si="1"/>
         <v>1.1000000000000001</v>
       </c>
@@ -5962,7 +5982,7 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8" s="25">
         <f t="shared" si="1"/>
         <v>0.45454545454545453</v>
       </c>
@@ -5994,7 +6014,7 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="E9" s="35">
+      <c r="E9" s="25">
         <f t="shared" si="1"/>
         <v>0.625</v>
       </c>
@@ -6030,7 +6050,7 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="E10" s="35">
+      <c r="E10" s="25">
         <f t="shared" si="1"/>
         <v>1.6</v>
       </c>
@@ -6062,7 +6082,7 @@
         <f t="shared" si="0"/>
         <v>117</v>
       </c>
-      <c r="E11" s="35">
+      <c r="E11" s="25">
         <f t="shared" si="1"/>
         <v>0.69230769230769229</v>
       </c>
@@ -6094,7 +6114,7 @@
         <f t="shared" si="0"/>
         <v>144</v>
       </c>
-      <c r="E12" s="35">
+      <c r="E12" s="25">
         <f t="shared" si="1"/>
         <v>1.7777777777777777</v>
       </c>
@@ -6126,7 +6146,7 @@
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="E13" s="35">
+      <c r="E13" s="25">
         <f t="shared" si="1"/>
         <v>1.1111111111111112</v>
       </c>
@@ -6158,7 +6178,7 @@
         <f t="shared" si="0"/>
         <v>156</v>
       </c>
-      <c r="E14" s="35">
+      <c r="E14" s="25">
         <f t="shared" si="1"/>
         <v>1.0833333333333333</v>
       </c>
@@ -6190,7 +6210,7 @@
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="E15" s="35">
+      <c r="E15" s="25">
         <f t="shared" si="1"/>
         <v>0.875</v>
       </c>
@@ -6222,7 +6242,7 @@
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="E16" s="35">
+      <c r="E16" s="25">
         <f t="shared" si="1"/>
         <v>0.88888888888888884</v>
       </c>
@@ -6254,7 +6274,7 @@
         <f t="shared" si="0"/>
         <v>130</v>
       </c>
-      <c r="E17" s="35">
+      <c r="E17" s="25">
         <f t="shared" si="1"/>
         <v>0.76923076923076927</v>
       </c>
@@ -6286,7 +6306,7 @@
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="E18" s="35">
+      <c r="E18" s="25">
         <f t="shared" si="1"/>
         <v>1.2857142857142858</v>
       </c>
@@ -6318,7 +6338,7 @@
         <f t="shared" si="0"/>
         <v>154</v>
       </c>
-      <c r="E19" s="35">
+      <c r="E19" s="25">
         <f t="shared" si="1"/>
         <v>1.2727272727272727</v>
       </c>
@@ -6350,7 +6370,7 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="E20" s="35">
+      <c r="E20" s="25">
         <f t="shared" si="1"/>
         <v>1.2</v>
       </c>
@@ -6382,7 +6402,7 @@
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="E21" s="35">
+      <c r="E21" s="25">
         <f t="shared" si="1"/>
         <v>1.875</v>
       </c>
@@ -6414,7 +6434,7 @@
         <f t="shared" si="0"/>
         <v>121</v>
       </c>
-      <c r="E22" s="35">
+      <c r="E22" s="25">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -6446,7 +6466,7 @@
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="E23" s="35">
+      <c r="E23" s="25">
         <f t="shared" si="1"/>
         <v>0.53333333333333333</v>
       </c>
@@ -6472,7 +6492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{553B0923-454E-41BC-A85D-BEF9AED5F553}">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -6497,52 +6517,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="7" t="s">
         <v>229</v>
       </c>
     </row>
@@ -6956,7 +6976,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="L12" s="38">
+      <c r="L12" s="28">
         <v>46146</v>
       </c>
     </row>
@@ -6975,8 +6995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F49CE1A-3C5C-49E9-8D0A-AD3DFF2EC16F}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6993,31 +7013,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>251</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>255</v>
       </c>
     </row>
@@ -7050,7 +7070,7 @@
         <f>IF(OR(B2&lt;33,C2&lt;33,D2&lt;33),"Fail","Pass")</f>
         <v>Fail</v>
       </c>
-      <c r="I2" s="35">
+      <c r="I2" s="25">
         <f>E2*100/300</f>
         <v>48.333333333333336</v>
       </c>
@@ -7084,7 +7104,7 @@
         <f t="shared" ref="H3:H10" si="3">IF(OR(B3&lt;33,C3&lt;33,D3&lt;33),"Fail","Pass")</f>
         <v>Fail</v>
       </c>
-      <c r="I3" s="35">
+      <c r="I3" s="25">
         <f t="shared" ref="I3:I10" si="4">E3*100/300</f>
         <v>46</v>
       </c>
@@ -7118,7 +7138,7 @@
         <f t="shared" si="3"/>
         <v>Fail</v>
       </c>
-      <c r="I4" s="35">
+      <c r="I4" s="25">
         <f t="shared" si="4"/>
         <v>59.333333333333336</v>
       </c>
@@ -7152,7 +7172,7 @@
         <f t="shared" si="3"/>
         <v>Pass</v>
       </c>
-      <c r="I5" s="35">
+      <c r="I5" s="25">
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
@@ -7186,7 +7206,7 @@
         <f t="shared" si="3"/>
         <v>Pass</v>
       </c>
-      <c r="I6" s="35">
+      <c r="I6" s="25">
         <f t="shared" si="4"/>
         <v>70.333333333333329</v>
       </c>
@@ -7220,7 +7240,7 @@
         <f t="shared" si="3"/>
         <v>Fail</v>
       </c>
-      <c r="I7" s="35">
+      <c r="I7" s="25">
         <f t="shared" si="4"/>
         <v>43.333333333333336</v>
       </c>
@@ -7254,7 +7274,7 @@
         <f t="shared" si="3"/>
         <v>Pass</v>
       </c>
-      <c r="I8" s="35">
+      <c r="I8" s="25">
         <f t="shared" si="4"/>
         <v>74</v>
       </c>
@@ -7288,7 +7308,7 @@
         <f t="shared" si="3"/>
         <v>Fail</v>
       </c>
-      <c r="I9" s="35">
+      <c r="I9" s="25">
         <f t="shared" si="4"/>
         <v>49.333333333333336</v>
       </c>
@@ -7322,7 +7342,7 @@
         <f t="shared" si="3"/>
         <v>Pass</v>
       </c>
-      <c r="I10" s="35">
+      <c r="I10" s="25">
         <f t="shared" si="4"/>
         <v>43</v>
       </c>

</xml_diff>